<commit_message>
Generated all mappings and navigator layers files
</commit_message>
<xml_diff>
--- a/src/mappings/groups/xlsx/veris-1_3_7-mappings-groups_v12.xlsx
+++ b/src/mappings/groups/xlsx/veris-1_3_7-mappings-groups_v12.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26216"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbergeron\Documents\_VERIS II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="482" documentId="13_ncr:1_{65AC85A1-C06D-44B5-93AB-7B325A1687BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0048FF3B-2189-4B5C-AE42-A0F9E683EB20}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15E1B5CF-874C-4EDD-B4CB-6419AFADBB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-50520" yWindow="285" windowWidth="25440" windowHeight="15390" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
   </bookViews>
@@ -2461,6 +2461,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date_x0020__x0026__x0020_Time xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <ProjectNum xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <TotalCost xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <Participants xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ec3e3de1-934b-464b-893a-587ae869df79" xsi:nil="true"/>
+    <MasterListID xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <ProjectName xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <CostPer xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010052D8A6B6F9FE2E45B0EDBAAD5FAF1312" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7022bf91ca57a9626808ed15fdcbfbd6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xmlns:ns3="ec3e3de1-934b-464b-893a-587ae869df79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d11a2dadb3f3bef5d5d1fdbc6ca57c91" ns2:_="" ns3:_="">
     <xsd:import namespace="0ca01121-da18-407e-86a0-e0ab1b6c7d8c"/>
@@ -2759,36 +2787,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date_x0020__x0026__x0020_Time xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <ProjectNum xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <TotalCost xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <Participants xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ec3e3de1-934b-464b-893a-587ae869df79" xsi:nil="true"/>
-    <MasterListID xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <ProjectName xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <CostPer xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{697EDC42-9C5C-463C-A7CA-B1F330E8878B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C05FA04D-3647-4F57-90F3-FA0A2E1CF7AC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2796,5 +2796,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C05FA04D-3647-4F57-90F3-FA0A2E1CF7AC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{697EDC42-9C5C-463C-A7CA-B1F330E8878B}"/>
 </file>
</xml_diff>